<commit_message>
Agregando archivos a la nueva rama
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\USCO\usco2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5975179-C593-4719-9CAB-A2446E0D56D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7952395D-2596-40B6-B5B7-E3A0BC4563CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB19E2A4-12D4-4992-BE8C-3F0D60C8381E}"/>
   </bookViews>
@@ -22,6 +22,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Hola Mundo</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,12 +379,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD63FFD-986D-4049-942E-462D3A195BE2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>